<commit_message>
Ramp is able to read excel
</commit_message>
<xml_diff>
--- a/ramp/input_files/test.xlsx
+++ b/ramp/input_files/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10427081_polimi_it/Documents/eNextGen/MARIO/MARIO U/Models/RAMP_modified/ramp/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="11_AD4DB114E441178AC67DF44CE6D4E0DA683EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20528548-CBCA-45CA-A5E9-0FBBA076ADAC}"/>
+  <xr:revisionPtr revIDLastSave="331" documentId="11_AD4DB114E441178AC67DF44CE6D4E0DA683EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42D4E605-1DFE-4F34-8DE5-23F729CD1B06}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
-  <si>
-    <t>Households</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>N. of windows</t>
   </si>
@@ -92,9 +89,6 @@
     <t>Weekend/weekday</t>
   </si>
   <si>
-    <t>Indoor_bulbs</t>
-  </si>
-  <si>
     <t>Window 1</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>Specific cycle 3</t>
   </si>
   <si>
-    <t>360,480</t>
-  </si>
-  <si>
     <t>Basic information</t>
   </si>
   <si>
@@ -144,6 +135,18 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>Church</t>
+  </si>
+  <si>
+    <t>Ch_indoor_bulb</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>1200,1400</t>
   </si>
 </sst>
 </file>
@@ -558,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,25 +572,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -599,11 +602,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4964AED-36AF-4373-9155-8099D6CFC5A9}">
   <dimension ref="A1:AH6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +631,7 @@
       <c r="A1" s="22"/>
       <c r="B1" s="22"/>
       <c r="C1" s="23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
@@ -643,27 +646,27 @@
       <c r="N1" s="23"/>
       <c r="O1" s="25"/>
       <c r="P1" s="23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="23"/>
       <c r="R1" s="23"/>
       <c r="S1" s="14"/>
       <c r="T1" s="24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="U1" s="23"/>
       <c r="V1" s="23"/>
       <c r="W1" s="23"/>
       <c r="X1" s="25"/>
       <c r="Y1" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="Z1" s="23"/>
       <c r="AA1" s="23"/>
       <c r="AB1" s="23"/>
       <c r="AC1" s="25"/>
       <c r="AD1" s="24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="AE1" s="23"/>
       <c r="AF1" s="23"/>
@@ -672,114 +675,114 @@
     </row>
     <row r="2" spans="1:34" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="I2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="16" t="s">
+      <c r="O2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="P2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="Q2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" s="18" t="s">
-        <v>21</v>
-      </c>
       <c r="S2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="T2" s="19" t="s">
+      <c r="U2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="U2" s="19" t="s">
+      <c r="W2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>29</v>
-      </c>
       <c r="X2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="19" t="s">
+      <c r="Z2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="19" t="s">
+      <c r="AB2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB2" s="19" t="s">
-        <v>29</v>
-      </c>
       <c r="AC2" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="AD2" s="19" t="s">
+      <c r="AE2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="AE2" s="19" t="s">
+      <c r="AG2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AF2" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG2" s="19" t="s">
-        <v>29</v>
-      </c>
       <c r="AH2" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -803,7 +806,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K3" s="3">
         <v>0</v>
@@ -812,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N3" s="3">
         <v>0</v>
@@ -821,13 +824,13 @@
         <v>2</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="S3" s="5">
         <v>0</v>
@@ -888,13 +891,13 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -902,12 +905,31 @@
       <c r="F5">
         <v>1</v>
       </c>
+      <c r="G5">
+        <v>210</v>
+      </c>
+      <c r="H5">
+        <v>0.2</v>
+      </c>
+      <c r="I5">
+        <v>60</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
       <c r="P5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="R5" s="12"/>
-      <c r="S5" s="9"/>
+      <c r="S5" s="9">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="P6" s="8"/>

</xml_diff>